<commit_message>
new template for cash disbursement
</commit_message>
<xml_diff>
--- a/public/files/Cash Disbursement Journal.xlsx
+++ b/public/files/Cash Disbursement Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>CASH DISBURSEMENT JOURNAL</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Month / Year</t>
+  </si>
+  <si>
+    <t>Repairs and Maintenance</t>
+  </si>
+  <si>
+    <t>Legal and Professional Expenses</t>
   </si>
 </sst>
 </file>
@@ -558,10 +564,10 @@
   <dimension ref="A1:AZ998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="AB6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A5"/>
+      <selection pane="bottomRight" activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -676,7 +682,7 @@
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
     </row>
-    <row r="4" spans="1:52" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -764,8 +770,12 @@
       <c r="AC4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AD4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
@@ -866,8 +876,12 @@
       <c r="AC5" s="10">
         <v>0</v>
       </c>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
+      <c r="AD5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="10">
+        <v>0</v>
+      </c>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>

</xml_diff>